<commit_message>
geolocation and map added
</commit_message>
<xml_diff>
--- a/Documents/addresses.xlsx
+++ b/Documents/addresses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,280 +424,336 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>CRA 70 # 26A - 33</t>
+          <t>CRA 97a # 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CRA 70 # 26A 33</t>
+          <t>CRA 97a # 2 70</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CRA 70 No 26A - 33</t>
+          <t>CRA 97a No 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CRA 70 No 26A 33</t>
+          <t>CRA 97a No 2 70</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CRA 70 Num 26A - 33</t>
+          <t>CRA 97a Num 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CRA 70 Num 26A 33</t>
+          <t>CRA 97a Num 2 70</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CRA 70 Numero 26A - 33</t>
+          <t>CRA 97a Numero 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CRA 70 Numero 26A 33</t>
+          <t>CRA 97a Numero 2 70</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kra 70 # 26A - 33</t>
+          <t>Carrera 97a # 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Kra 70 # 26A 33</t>
+          <t>Carrera 97a # 2 70</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Kra 70 No 26A - 33</t>
+          <t>Carrera 97a No 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Kra 70 No 26A 33</t>
+          <t>Carrera 97a No 2 70</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Kra 70 Num 26A - 33</t>
+          <t>Carrera 97a Num 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Kra 70 Num 26A 33</t>
+          <t>Carrera 97a Num 2 70</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Kra 70 Numero 26A - 33</t>
+          <t>Carrera 97a Numero 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Kra 70 Numero 26A 33</t>
+          <t>Carrera 97a Numero 2 70</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Carrera 70 # 26A - 33</t>
+          <t>Calle 97a # 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Carrera 70 # 26A 33</t>
+          <t>Calle 97a # 2 70</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Carrera 70 No 26A - 33</t>
+          <t>Calle 97a No 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Carrera 70 No 26A 33</t>
+          <t>Calle 97a No 2 70</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Carrera 70 Num 26A - 33</t>
+          <t>Calle 97a Num 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Carrera 70 Num 26A 33</t>
+          <t>Calle 97a Num 2 70</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Carrera 70 Numero 26A - 33</t>
+          <t>Calle 97a Numero 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Carrera 70 Numero 26A 33</t>
+          <t>Calle 97a Numero 2 70</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Calle 70 # 26A - 33</t>
+          <t>Cl 97a # 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Calle 70 # 26A 33</t>
+          <t>Cl 97a # 2 70</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Calle 70 No 26A - 33</t>
+          <t>Cl 97a No 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Calle 70 No 26A 33</t>
+          <t>Cl 97a No 2 70</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Calle 70 Num 26A - 33</t>
+          <t>Cl 97a Num 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Calle 70 Num 26A 33</t>
+          <t>Cl 97a Num 2 70</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Calle 70 Numero 26A - 33</t>
+          <t>Cl 97a Numero 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Calle 70 Numero 26A 33</t>
+          <t>Cl 97a Numero 2 70</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Transversal 70 # 26A - 33</t>
+          <t>Transversal 97a # 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Transversal 70 # 26A 33</t>
+          <t>Transversal 97a # 2 70</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Transversal 70 No 26A - 33</t>
+          <t>Transversal 97a No 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Transversal 70 No 26A 33</t>
+          <t>Transversal 97a No 2 70</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Transversal 70 Num 26A - 33</t>
+          <t>Transversal 97a Num 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Transversal 70 Num 26A 33</t>
+          <t>Transversal 97a Num 2 70</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Transversal 70 Numero 26A - 33</t>
+          <t>Transversal 97a Numero 2 - 70</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Transversal 70 Numero 26A 33</t>
+          <t>Transversal 97a Numero 2 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Tv 97a # 2 - 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Tv 97a # 2 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Tv 97a No 2 - 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Tv 97a No 2 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Tv 97a Num 2 - 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Tv 97a Num 2 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Tv 97a Numero 2 - 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Tv 97a Numero 2 70</t>
         </is>
       </c>
     </row>

</xml_diff>